<commit_message>
Color sensor code 1
</commit_message>
<xml_diff>
--- a/LogBook.xlsx
+++ b/LogBook.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TUe\EmbeddedSystems\CBLEmbeded\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kings\Desktop\Embedded\CBLEmbeded\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85563C7E-2948-4606-8828-2B41CFE167CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F4D3359-3C34-4954-A6EB-9F3476B37541}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7800" yWindow="2250" windowWidth="17280" windowHeight="8994" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -57,7 +57,7 @@
     <t>Trayana ()</t>
   </si>
   <si>
-    <t>Hristo ()</t>
+    <t>Hristo (1940651)</t>
   </si>
 </sst>
 </file>
@@ -321,9 +321,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -342,9 +339,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -361,28 +355,22 @@
     <xf numFmtId="14" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -391,21 +379,33 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Нормален" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -686,18 +686,18 @@
   <dimension ref="A1:D45"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="A28" sqref="A28:A33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="24.89453125" customWidth="1"/>
-    <col min="2" max="2" width="47.83984375" customWidth="1"/>
-    <col min="3" max="3" width="24.47265625" customWidth="1"/>
-    <col min="4" max="4" width="17.62890625" customWidth="1"/>
+    <col min="1" max="1" width="24.88671875" customWidth="1"/>
+    <col min="2" max="2" width="47.88671875" customWidth="1"/>
+    <col min="3" max="3" width="24.44140625" customWidth="1"/>
+    <col min="4" max="4" width="17.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -711,283 +711,283 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="5" t="s">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="6"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="8"/>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" s="5"/>
-      <c r="B3" s="9"/>
-      <c r="C3" s="10"/>
-      <c r="D3" s="11"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" s="12"/>
-      <c r="B4" s="13"/>
-      <c r="C4" s="14"/>
-      <c r="D4" s="15"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" s="12"/>
-      <c r="B5" s="16"/>
-      <c r="C5" s="17"/>
-      <c r="D5" s="11"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" s="12"/>
-      <c r="B6" s="13"/>
-      <c r="C6" s="18"/>
-      <c r="D6" s="11"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7" s="12"/>
-      <c r="B7" s="13"/>
-      <c r="C7" s="14"/>
-      <c r="D7" s="11"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8" s="19"/>
-      <c r="B8" s="13"/>
-      <c r="C8" s="18"/>
-      <c r="D8" s="11"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A9" s="20" t="s">
+      <c r="B2" s="5"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="7"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="25"/>
+      <c r="B3" s="8"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="10"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="26"/>
+      <c r="B4" s="11"/>
+      <c r="C4" s="12"/>
+      <c r="D4" s="13"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="26"/>
+      <c r="B5" s="14"/>
+      <c r="C5" s="15"/>
+      <c r="D5" s="10"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="26"/>
+      <c r="B6" s="11"/>
+      <c r="C6" s="16"/>
+      <c r="D6" s="10"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="26"/>
+      <c r="B7" s="11"/>
+      <c r="C7" s="12"/>
+      <c r="D7" s="10"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="27"/>
+      <c r="B8" s="11"/>
+      <c r="C8" s="16"/>
+      <c r="D8" s="10"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="21"/>
-      <c r="C9" s="22"/>
-      <c r="D9" s="8"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A10" s="23"/>
-      <c r="B10" s="16"/>
-      <c r="C10" s="14"/>
-      <c r="D10" s="11"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A11" s="23"/>
-      <c r="B11" s="16"/>
-      <c r="C11" s="14"/>
-      <c r="D11" s="11"/>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A12" s="23"/>
-      <c r="B12" s="16"/>
-      <c r="C12" s="14"/>
-      <c r="D12" s="11"/>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A13" s="23"/>
-      <c r="B13" s="16"/>
-      <c r="C13" s="14"/>
-      <c r="D13" s="11"/>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A14" s="23"/>
-      <c r="B14" s="16"/>
-      <c r="C14" s="14"/>
-      <c r="D14" s="11"/>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A15" s="24" t="s">
+      <c r="B9" s="17"/>
+      <c r="C9" s="18"/>
+      <c r="D9" s="7"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="29"/>
+      <c r="B10" s="14"/>
+      <c r="C10" s="12"/>
+      <c r="D10" s="10"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" s="29"/>
+      <c r="B11" s="14"/>
+      <c r="C11" s="12"/>
+      <c r="D11" s="10"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" s="29"/>
+      <c r="B12" s="14"/>
+      <c r="C12" s="12"/>
+      <c r="D12" s="10"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" s="29"/>
+      <c r="B13" s="14"/>
+      <c r="C13" s="12"/>
+      <c r="D13" s="10"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" s="29"/>
+      <c r="B14" s="14"/>
+      <c r="C14" s="12"/>
+      <c r="D14" s="10"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="B15" s="21"/>
-      <c r="C15" s="22"/>
-      <c r="D15" s="8"/>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A16" s="25"/>
-      <c r="B16" s="16"/>
-      <c r="C16" s="14"/>
-      <c r="D16" s="11"/>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A17" s="25"/>
-      <c r="B17" s="16"/>
-      <c r="C17" s="14"/>
-      <c r="D17" s="11"/>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A18" s="25"/>
-      <c r="B18" s="16"/>
-      <c r="C18" s="14"/>
-      <c r="D18" s="11"/>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A19" s="25"/>
-      <c r="B19" s="16"/>
-      <c r="C19" s="14"/>
-      <c r="D19" s="11"/>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A20" s="25"/>
-      <c r="B20" s="16"/>
-      <c r="C20" s="14"/>
-      <c r="D20" s="11"/>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A21" s="26"/>
-      <c r="B21" s="16"/>
-      <c r="C21" s="14"/>
-      <c r="D21" s="11"/>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A22" s="27" t="s">
+      <c r="B15" s="17"/>
+      <c r="C15" s="18"/>
+      <c r="D15" s="7"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" s="31"/>
+      <c r="B16" s="14"/>
+      <c r="C16" s="12"/>
+      <c r="D16" s="10"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" s="31"/>
+      <c r="B17" s="14"/>
+      <c r="C17" s="12"/>
+      <c r="D17" s="10"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" s="31"/>
+      <c r="B18" s="14"/>
+      <c r="C18" s="12"/>
+      <c r="D18" s="10"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" s="31"/>
+      <c r="B19" s="14"/>
+      <c r="C19" s="12"/>
+      <c r="D19" s="10"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" s="31"/>
+      <c r="B20" s="14"/>
+      <c r="C20" s="12"/>
+      <c r="D20" s="10"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" s="32"/>
+      <c r="B21" s="14"/>
+      <c r="C21" s="12"/>
+      <c r="D21" s="10"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="B22" s="21"/>
-      <c r="C22" s="22"/>
-      <c r="D22" s="8"/>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A23" s="28"/>
-      <c r="B23" s="16"/>
-      <c r="C23" s="14"/>
-      <c r="D23" s="11"/>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A24" s="28"/>
-      <c r="B24" s="16"/>
-      <c r="C24" s="14"/>
-      <c r="D24" s="11"/>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A25" s="28"/>
-      <c r="B25" s="16"/>
-      <c r="C25" s="29"/>
-      <c r="D25" s="11"/>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A26" s="28"/>
-      <c r="B26" s="16"/>
-      <c r="C26" s="29"/>
-      <c r="D26" s="11"/>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A27" s="28"/>
-      <c r="B27" s="30"/>
-      <c r="C27" s="31"/>
-      <c r="D27" s="32"/>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A28" s="27" t="s">
+      <c r="B22" s="17"/>
+      <c r="C22" s="18"/>
+      <c r="D22" s="7"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23" s="24"/>
+      <c r="B23" s="14"/>
+      <c r="C23" s="12"/>
+      <c r="D23" s="10"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24" s="24"/>
+      <c r="B24" s="14"/>
+      <c r="C24" s="12"/>
+      <c r="D24" s="10"/>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25" s="24"/>
+      <c r="B25" s="14"/>
+      <c r="C25" s="19"/>
+      <c r="D25" s="10"/>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A26" s="24"/>
+      <c r="B26" s="14"/>
+      <c r="C26" s="19"/>
+      <c r="D26" s="10"/>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A27" s="24"/>
+      <c r="B27" s="20"/>
+      <c r="C27" s="21"/>
+      <c r="D27" s="22"/>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A28" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="B28" s="21"/>
-      <c r="C28" s="22"/>
-      <c r="D28" s="8"/>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A29" s="28"/>
-      <c r="B29" s="16"/>
-      <c r="C29" s="14"/>
-      <c r="D29" s="11"/>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A30" s="28"/>
-      <c r="B30" s="16"/>
-      <c r="C30" s="14"/>
-      <c r="D30" s="11"/>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A31" s="28"/>
-      <c r="B31" s="16"/>
-      <c r="C31" s="29"/>
-      <c r="D31" s="11"/>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A32" s="28"/>
-      <c r="B32" s="16"/>
-      <c r="C32" s="29"/>
-      <c r="D32" s="11"/>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A33" s="28"/>
-      <c r="B33" s="30"/>
-      <c r="C33" s="31"/>
-      <c r="D33" s="32"/>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A34" s="27" t="s">
+      <c r="B28" s="17"/>
+      <c r="C28" s="18"/>
+      <c r="D28" s="7"/>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A29" s="24"/>
+      <c r="B29" s="14"/>
+      <c r="C29" s="12"/>
+      <c r="D29" s="10"/>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A30" s="24"/>
+      <c r="B30" s="14"/>
+      <c r="C30" s="12"/>
+      <c r="D30" s="10"/>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A31" s="24"/>
+      <c r="B31" s="14"/>
+      <c r="C31" s="19"/>
+      <c r="D31" s="10"/>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A32" s="24"/>
+      <c r="B32" s="14"/>
+      <c r="C32" s="19"/>
+      <c r="D32" s="10"/>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A33" s="24"/>
+      <c r="B33" s="20"/>
+      <c r="C33" s="21"/>
+      <c r="D33" s="22"/>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A34" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="B34" s="21"/>
-      <c r="C34" s="22"/>
-      <c r="D34" s="8"/>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A35" s="28"/>
-      <c r="B35" s="16"/>
-      <c r="C35" s="14"/>
-      <c r="D35" s="11"/>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A36" s="28"/>
-      <c r="B36" s="16"/>
-      <c r="C36" s="14"/>
-      <c r="D36" s="11"/>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A37" s="28"/>
-      <c r="B37" s="16"/>
-      <c r="C37" s="29"/>
-      <c r="D37" s="11"/>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A38" s="28"/>
-      <c r="B38" s="16"/>
-      <c r="C38" s="29"/>
-      <c r="D38" s="11"/>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A39" s="28"/>
-      <c r="B39" s="30"/>
-      <c r="C39" s="31"/>
-      <c r="D39" s="32"/>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A40" s="27" t="s">
+      <c r="B34" s="17"/>
+      <c r="C34" s="18"/>
+      <c r="D34" s="7"/>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A35" s="24"/>
+      <c r="B35" s="14"/>
+      <c r="C35" s="12"/>
+      <c r="D35" s="10"/>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A36" s="24"/>
+      <c r="B36" s="14"/>
+      <c r="C36" s="12"/>
+      <c r="D36" s="10"/>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A37" s="24"/>
+      <c r="B37" s="14"/>
+      <c r="C37" s="19"/>
+      <c r="D37" s="10"/>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A38" s="24"/>
+      <c r="B38" s="14"/>
+      <c r="C38" s="19"/>
+      <c r="D38" s="10"/>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A39" s="24"/>
+      <c r="B39" s="20"/>
+      <c r="C39" s="21"/>
+      <c r="D39" s="22"/>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A40" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="B40" s="21"/>
-      <c r="C40" s="22"/>
-      <c r="D40" s="8"/>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A41" s="28"/>
-      <c r="B41" s="16"/>
-      <c r="C41" s="14"/>
-      <c r="D41" s="11"/>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A42" s="28"/>
-      <c r="B42" s="16"/>
-      <c r="C42" s="14"/>
-      <c r="D42" s="11"/>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A43" s="28"/>
-      <c r="B43" s="16"/>
-      <c r="C43" s="29"/>
-      <c r="D43" s="11"/>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A44" s="28"/>
-      <c r="B44" s="16"/>
-      <c r="C44" s="29"/>
-      <c r="D44" s="11"/>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A45" s="28"/>
-      <c r="B45" s="30"/>
-      <c r="C45" s="31"/>
-      <c r="D45" s="32"/>
+      <c r="B40" s="17"/>
+      <c r="C40" s="18"/>
+      <c r="D40" s="7"/>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A41" s="24"/>
+      <c r="B41" s="14"/>
+      <c r="C41" s="12"/>
+      <c r="D41" s="10"/>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A42" s="24"/>
+      <c r="B42" s="14"/>
+      <c r="C42" s="12"/>
+      <c r="D42" s="10"/>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A43" s="24"/>
+      <c r="B43" s="14"/>
+      <c r="C43" s="19"/>
+      <c r="D43" s="10"/>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A44" s="24"/>
+      <c r="B44" s="14"/>
+      <c r="C44" s="19"/>
+      <c r="D44" s="10"/>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A45" s="24"/>
+      <c r="B45" s="20"/>
+      <c r="C45" s="21"/>
+      <c r="D45" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="7">

</xml_diff>